<commit_message>
Add TermListVocab.present_in_version? & .not_yet_loaded? methods
</commit_message>
<xml_diff>
--- a/spec/support/fixtures/shared_term_lists.xlsx
+++ b/spec/support/fixtures/shared_term_lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristina/code/cs/migration_tools/spec/support/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC97F6B-AE9C-3F4E-B3CE-A6192B6A6968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA3518E-095B-E04D-B701-7255A874DFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="129">
   <si>
     <t>term_list_displayName</t>
   </si>
@@ -408,6 +408,21 @@
   </si>
   <si>
     <t>termStatus</t>
+  </si>
+  <si>
+    <t>New Vocab</t>
+  </si>
+  <si>
+    <t>newvocab</t>
+  </si>
+  <si>
+    <t>Term 1</t>
+  </si>
+  <si>
+    <t>Term 2</t>
+  </si>
+  <si>
+    <t>Term 3</t>
   </si>
 </sst>
 </file>
@@ -455,9 +470,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,8 +496,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A345EA12-E723-8C4C-9C3A-51BA5560AEBE}" name="termData" displayName="termData" ref="A1:L73" totalsRowShown="0">
-  <autoFilter ref="A1:L73" xr:uid="{A345EA12-E723-8C4C-9C3A-51BA5560AEBE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A345EA12-E723-8C4C-9C3A-51BA5560AEBE}" name="termData" displayName="termData" ref="A1:L76" totalsRowShown="0">
+  <autoFilter ref="A1:L76" xr:uid="{A345EA12-E723-8C4C-9C3A-51BA5560AEBE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L73">
     <sortCondition ref="G1:G73"/>
   </sortState>
@@ -824,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="L75" sqref="L75:L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2866,6 +2882,90 @@
       </c>
       <c r="L73" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,E74,L74)</f>
+        <v>newvocab Term 1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>124</v>
+      </c>
+      <c r="E74" t="s">
+        <v>125</v>
+      </c>
+      <c r="F74" t="s">
+        <v>126</v>
+      </c>
+      <c r="K74" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,C74,A74)</f>
+        <v>newvocab Term 1 4</v>
+      </c>
+      <c r="L74" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,E75,L75)</f>
+        <v>newvocab Term 2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>124</v>
+      </c>
+      <c r="E75" t="s">
+        <v>125</v>
+      </c>
+      <c r="F75" t="s">
+        <v>127</v>
+      </c>
+      <c r="K75" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,C75,A75)</f>
+        <v>newvocab Term 2 4</v>
+      </c>
+      <c r="L75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>4</v>
+      </c>
+      <c r="B76" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,E76,L76)</f>
+        <v>newvocab Term 3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>124</v>
+      </c>
+      <c r="E76" t="s">
+        <v>125</v>
+      </c>
+      <c r="F76" t="s">
+        <v>128</v>
+      </c>
+      <c r="K76" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,C76,A76)</f>
+        <v>newvocab Term 3 4</v>
+      </c>
+      <c r="L76" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test: Update dynamic term list fixture to match current format
</commit_message>
<xml_diff>
--- a/spec/support/fixtures/shared_term_lists.xlsx
+++ b/spec/support/fixtures/shared_term_lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristina/code/cs/migration_tools/spec/support/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA3518E-095B-E04D-B701-7255A874DFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49478766-F2E2-4547-A0E3-11C984C8AADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="10800" windowWidth="38400" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="termData" sheetId="1" r:id="rId1"/>
@@ -395,9 +395,6 @@
     <t>stone, unmodified</t>
   </si>
   <si>
-    <t>displayName</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -423,6 +420,9 @@
   </si>
   <si>
     <t>Term 3</t>
+  </si>
+  <si>
+    <t>term</t>
   </si>
 </sst>
 </file>
@@ -470,10 +470,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +508,7 @@
     </tableColumn>
     <tableColumn id="4" xr3:uid="{67D87138-A73D-0E42-BE6C-5D8BAEE62A4A}" name="term_list_displayName"/>
     <tableColumn id="5" xr3:uid="{9DD330C3-2932-0640-AB21-F4B9466216C9}" name="term_list_shortIdentifier"/>
-    <tableColumn id="6" xr3:uid="{32AD7F31-7CD0-5249-B1AD-67EE775A1195}" name="displayName"/>
+    <tableColumn id="6" xr3:uid="{32AD7F31-7CD0-5249-B1AD-67EE775A1195}" name="term"/>
     <tableColumn id="7" xr3:uid="{6429C7D4-94B4-EF4C-AC41-947864AD3761}" name="description"/>
     <tableColumn id="10" xr3:uid="{64D8C81E-E305-5045-ACB9-5F2C2E1341CC}" name="source"/>
     <tableColumn id="11" xr3:uid="{924351F6-467D-FB44-AAE4-57EFDD4733DB}" name="sourcePage"/>
@@ -842,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="L75" sqref="L75:L76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -873,19 +872,19 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" t="s">
         <v>119</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>120</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>121</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>122</v>
-      </c>
-      <c r="J1" t="s">
-        <v>123</v>
       </c>
       <c r="K1" t="s">
         <v>73</v>
@@ -902,7 +901,7 @@
         <v>72</v>
       </c>
       <c r="C2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E2,L2)</f>
+        <f t="shared" ref="C2:C24" si="0">_xlfn.TEXTJOIN(" ",TRUE,E2,L2)</f>
         <v>nagpracategory associated funerary object (AFO)</v>
       </c>
       <c r="D2" t="s">
@@ -915,7 +914,7 @@
         <v>20</v>
       </c>
       <c r="K2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C2,A2)</f>
+        <f t="shared" ref="K2:K24" si="1">_xlfn.TEXTJOIN(" ",TRUE,C2,A2)</f>
         <v>nagpracategory associated funerary object (AFO) 0</v>
       </c>
       <c r="L2" t="s">
@@ -930,7 +929,7 @@
         <v>72</v>
       </c>
       <c r="C3" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E3,L3)</f>
+        <f t="shared" si="0"/>
         <v>nagpracategory human remains</v>
       </c>
       <c r="D3" t="s">
@@ -943,7 +942,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C3,A3)</f>
+        <f t="shared" si="1"/>
         <v>nagpracategory human remains 0</v>
       </c>
       <c r="L3" t="s">
@@ -958,7 +957,7 @@
         <v>72</v>
       </c>
       <c r="C4" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E4,L4)</f>
+        <f t="shared" si="0"/>
         <v>nagpracategory object of cultural patrimony</v>
       </c>
       <c r="D4" t="s">
@@ -971,7 +970,7 @@
         <v>22</v>
       </c>
       <c r="K4" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C4,A4)</f>
+        <f t="shared" si="1"/>
         <v>nagpracategory object of cultural patrimony 0</v>
       </c>
       <c r="L4" t="s">
@@ -986,7 +985,7 @@
         <v>72</v>
       </c>
       <c r="C5" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E5,L5)</f>
+        <f t="shared" si="0"/>
         <v>nagpracategory sacred object</v>
       </c>
       <c r="D5" t="s">
@@ -999,7 +998,7 @@
         <v>23</v>
       </c>
       <c r="K5" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C5,A5)</f>
+        <f t="shared" si="1"/>
         <v>nagpracategory sacred object 0</v>
       </c>
       <c r="L5" t="s">
@@ -1014,7 +1013,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E6,L6)</f>
+        <f t="shared" si="0"/>
         <v>nagpracategory subject to NAGPRA, unspecified</v>
       </c>
       <c r="D6" t="s">
@@ -1027,7 +1026,7 @@
         <v>24</v>
       </c>
       <c r="K6" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C6,A6)</f>
+        <f t="shared" si="1"/>
         <v>nagpracategory subject to NAGPRA, unspecified 0</v>
       </c>
       <c r="L6" t="s">
@@ -1042,7 +1041,7 @@
         <v>72</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E7,L7)</f>
+        <f t="shared" si="0"/>
         <v>nagpracategory unassociated funerary object (UFO)</v>
       </c>
       <c r="D7" t="s">
@@ -1055,7 +1054,7 @@
         <v>25</v>
       </c>
       <c r="K7" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C7,A7)</f>
+        <f t="shared" si="1"/>
         <v>nagpracategory unassociated funerary object (UFO) 0</v>
       </c>
       <c r="L7" t="s">
@@ -1070,7 +1069,7 @@
         <v>72</v>
       </c>
       <c r="C8" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E8,L8)</f>
+        <f t="shared" si="0"/>
         <v>nagpraclaimtype associated funerary object (AFO)</v>
       </c>
       <c r="D8" t="s">
@@ -1083,7 +1082,7 @@
         <v>20</v>
       </c>
       <c r="K8" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C8,A8)</f>
+        <f t="shared" si="1"/>
         <v>nagpraclaimtype associated funerary object (AFO) 0</v>
       </c>
       <c r="L8" t="s">
@@ -1098,7 +1097,7 @@
         <v>72</v>
       </c>
       <c r="C9" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E9,L9)</f>
+        <f t="shared" si="0"/>
         <v>nagpraclaimtype human remains</v>
       </c>
       <c r="D9" t="s">
@@ -1111,7 +1110,7 @@
         <v>21</v>
       </c>
       <c r="K9" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C9,A9)</f>
+        <f t="shared" si="1"/>
         <v>nagpraclaimtype human remains 0</v>
       </c>
       <c r="L9" t="s">
@@ -1126,7 +1125,7 @@
         <v>72</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E10,L10)</f>
+        <f t="shared" si="0"/>
         <v>nagpraclaimtype object of cultural patrimony</v>
       </c>
       <c r="D10" t="s">
@@ -1139,7 +1138,7 @@
         <v>22</v>
       </c>
       <c r="K10" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C10,A10)</f>
+        <f t="shared" si="1"/>
         <v>nagpraclaimtype object of cultural patrimony 0</v>
       </c>
       <c r="L10" t="s">
@@ -1154,7 +1153,7 @@
         <v>72</v>
       </c>
       <c r="C11" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E11,L11)</f>
+        <f t="shared" si="0"/>
         <v>nagpraclaimtype sacred object</v>
       </c>
       <c r="D11" t="s">
@@ -1167,7 +1166,7 @@
         <v>23</v>
       </c>
       <c r="K11" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C11,A11)</f>
+        <f t="shared" si="1"/>
         <v>nagpraclaimtype sacred object 0</v>
       </c>
       <c r="L11" t="s">
@@ -1182,7 +1181,7 @@
         <v>72</v>
       </c>
       <c r="C12" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E12,L12)</f>
+        <f t="shared" si="0"/>
         <v>nagpraclaimtype unassociated funerary object (UFO)</v>
       </c>
       <c r="D12" t="s">
@@ -1195,7 +1194,7 @@
         <v>25</v>
       </c>
       <c r="K12" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C12,A12)</f>
+        <f t="shared" si="1"/>
         <v>nagpraclaimtype unassociated funerary object (UFO) 0</v>
       </c>
       <c r="L12" t="s">
@@ -1210,7 +1209,7 @@
         <v>72</v>
       </c>
       <c r="C13" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E13,L13)</f>
+        <f t="shared" si="0"/>
         <v>nagpraclaimtype unrelated to NAGPRA</v>
       </c>
       <c r="D13" t="s">
@@ -1223,7 +1222,7 @@
         <v>29</v>
       </c>
       <c r="K13" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C13,A13)</f>
+        <f t="shared" si="1"/>
         <v>nagpraclaimtype unrelated to NAGPRA 0</v>
       </c>
       <c r="L13" t="s">
@@ -1238,7 +1237,7 @@
         <v>72</v>
       </c>
       <c r="C14" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E14,L14)</f>
+        <f t="shared" si="0"/>
         <v>nagprainventory inventory, complete</v>
       </c>
       <c r="D14" t="s">
@@ -1251,7 +1250,7 @@
         <v>32</v>
       </c>
       <c r="K14" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C14,A14)</f>
+        <f t="shared" si="1"/>
         <v>nagprainventory inventory, complete 0</v>
       </c>
       <c r="L14" t="s">
@@ -1266,7 +1265,7 @@
         <v>72</v>
       </c>
       <c r="C15" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E15,L15)</f>
+        <f t="shared" si="0"/>
         <v>nagprainventory inventory, in progress</v>
       </c>
       <c r="D15" t="s">
@@ -1279,7 +1278,7 @@
         <v>33</v>
       </c>
       <c r="K15" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C15,A15)</f>
+        <f t="shared" si="1"/>
         <v>nagprainventory inventory, in progress 0</v>
       </c>
       <c r="L15" t="s">
@@ -1294,7 +1293,7 @@
         <v>72</v>
       </c>
       <c r="C16" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E16,L16)</f>
+        <f t="shared" si="0"/>
         <v>nagprainventory inventory, not started</v>
       </c>
       <c r="D16" t="s">
@@ -1307,7 +1306,7 @@
         <v>34</v>
       </c>
       <c r="K16" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C16,A16)</f>
+        <f t="shared" si="1"/>
         <v>nagprainventory inventory, not started 0</v>
       </c>
       <c r="L16" t="s">
@@ -1322,7 +1321,7 @@
         <v>72</v>
       </c>
       <c r="C17" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E17,L17)</f>
+        <f t="shared" si="0"/>
         <v>nagprainventory summary, complete</v>
       </c>
       <c r="D17" t="s">
@@ -1335,7 +1334,7 @@
         <v>35</v>
       </c>
       <c r="K17" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C17,A17)</f>
+        <f t="shared" si="1"/>
         <v>nagprainventory summary, complete 0</v>
       </c>
       <c r="L17" t="s">
@@ -1350,7 +1349,7 @@
         <v>72</v>
       </c>
       <c r="C18" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E18,L18)</f>
+        <f t="shared" si="0"/>
         <v>nagprainventory summary, in progress</v>
       </c>
       <c r="D18" t="s">
@@ -1363,7 +1362,7 @@
         <v>36</v>
       </c>
       <c r="K18" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C18,A18)</f>
+        <f t="shared" si="1"/>
         <v>nagprainventory summary, in progress 0</v>
       </c>
       <c r="L18" t="s">
@@ -1378,7 +1377,7 @@
         <v>72</v>
       </c>
       <c r="C19" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E19,L19)</f>
+        <f t="shared" si="0"/>
         <v>nagprainventory summary, not started</v>
       </c>
       <c r="D19" t="s">
@@ -1391,7 +1390,7 @@
         <v>37</v>
       </c>
       <c r="K19" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C19,A19)</f>
+        <f t="shared" si="1"/>
         <v>nagprainventory summary, not started 0</v>
       </c>
       <c r="L19" t="s">
@@ -1406,7 +1405,7 @@
         <v>72</v>
       </c>
       <c r="C20" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E20,L20)</f>
+        <f t="shared" si="0"/>
         <v>objectcategory debitage</v>
       </c>
       <c r="D20" t="s">
@@ -1419,7 +1418,7 @@
         <v>41</v>
       </c>
       <c r="K20" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C20,A20)</f>
+        <f t="shared" si="1"/>
         <v>objectcategory debitage 0</v>
       </c>
       <c r="L20" t="s">
@@ -1434,7 +1433,7 @@
         <v>72</v>
       </c>
       <c r="C21" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E21,L21)</f>
+        <f t="shared" si="0"/>
         <v>objectcategory ethnographic</v>
       </c>
       <c r="D21" t="s">
@@ -1447,7 +1446,7 @@
         <v>42</v>
       </c>
       <c r="K21" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C21,A21)</f>
+        <f t="shared" si="1"/>
         <v>objectcategory ethnographic 0</v>
       </c>
       <c r="L21" t="s">
@@ -1462,7 +1461,7 @@
         <v>72</v>
       </c>
       <c r="C22" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E22,L22)</f>
+        <f t="shared" si="0"/>
         <v>objectcategory historics</v>
       </c>
       <c r="D22" t="s">
@@ -1475,7 +1474,7 @@
         <v>43</v>
       </c>
       <c r="K22" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C22,A22)</f>
+        <f t="shared" si="1"/>
         <v>objectcategory historics 0</v>
       </c>
       <c r="L22" t="s">
@@ -1490,7 +1489,7 @@
         <v>72</v>
       </c>
       <c r="C23" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E23,L23)</f>
+        <f t="shared" si="0"/>
         <v>objectcategory human remains</v>
       </c>
       <c r="D23" t="s">
@@ -1503,7 +1502,7 @@
         <v>21</v>
       </c>
       <c r="K23" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C23,A23)</f>
+        <f t="shared" si="1"/>
         <v>objectcategory human remains 0</v>
       </c>
       <c r="L23" t="s">
@@ -1518,7 +1517,7 @@
         <v>72</v>
       </c>
       <c r="C24" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E24,L24)</f>
+        <f t="shared" si="0"/>
         <v>objectcategory modified faunal remains</v>
       </c>
       <c r="D24" t="s">
@@ -1531,7 +1530,7 @@
         <v>44</v>
       </c>
       <c r="K24" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C24,A24)</f>
+        <f t="shared" si="1"/>
         <v>objectcategory modified faunal remains 0</v>
       </c>
       <c r="L24" t="s">
@@ -2140,7 +2139,7 @@
         <v>72</v>
       </c>
       <c r="C47" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E47,L47)</f>
+        <f t="shared" ref="C47:C58" si="2">_xlfn.TEXTJOIN(" ",TRUE,E47,L47)</f>
         <v>annotationtype cataloging note</v>
       </c>
       <c r="D47" t="s">
@@ -2153,7 +2152,7 @@
         <v>4</v>
       </c>
       <c r="K47" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C47,A47)</f>
+        <f t="shared" ref="K47:K58" si="3">_xlfn.TEXTJOIN(" ",TRUE,C47,A47)</f>
         <v>annotationtype cataloging note 0</v>
       </c>
       <c r="L47" t="s">
@@ -2168,7 +2167,7 @@
         <v>72</v>
       </c>
       <c r="C48" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E48,L48)</f>
+        <f t="shared" si="2"/>
         <v>annotationtype migration note</v>
       </c>
       <c r="D48" t="s">
@@ -2181,7 +2180,7 @@
         <v>5</v>
       </c>
       <c r="K48" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C48,A48)</f>
+        <f t="shared" si="3"/>
         <v>annotationtype migration note 0</v>
       </c>
       <c r="L48" t="s">
@@ -2196,7 +2195,7 @@
         <v>72</v>
       </c>
       <c r="C49" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E49,L49)</f>
+        <f t="shared" si="2"/>
         <v>annotationtype staff note</v>
       </c>
       <c r="D49" t="s">
@@ -2209,7 +2208,7 @@
         <v>6</v>
       </c>
       <c r="K49" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C49,A49)</f>
+        <f t="shared" si="3"/>
         <v>annotationtype staff note 0</v>
       </c>
       <c r="L49" t="s">
@@ -2224,7 +2223,7 @@
         <v>72</v>
       </c>
       <c r="C50" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E50,L50)</f>
+        <f t="shared" si="2"/>
         <v>descriptionlevel collection</v>
       </c>
       <c r="D50" t="s">
@@ -2237,7 +2236,7 @@
         <v>9</v>
       </c>
       <c r="K50" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C50,A50)</f>
+        <f t="shared" si="3"/>
         <v>descriptionlevel collection 0</v>
       </c>
       <c r="L50" t="s">
@@ -2252,7 +2251,7 @@
         <v>72</v>
       </c>
       <c r="C51" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E51,L51)</f>
+        <f t="shared" si="2"/>
         <v>descriptionlevel individual remains or cultural object</v>
       </c>
       <c r="D51" t="s">
@@ -2265,7 +2264,7 @@
         <v>10</v>
       </c>
       <c r="K51" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C51,A51)</f>
+        <f t="shared" si="3"/>
         <v>descriptionlevel individual remains or cultural object 0</v>
       </c>
       <c r="L51" t="s">
@@ -2280,7 +2279,7 @@
         <v>72</v>
       </c>
       <c r="C52" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E52,L52)</f>
+        <f t="shared" si="2"/>
         <v>descriptionlevel supporting collection</v>
       </c>
       <c r="D52" t="s">
@@ -2293,7 +2292,7 @@
         <v>11</v>
       </c>
       <c r="K52" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C52,A52)</f>
+        <f t="shared" si="3"/>
         <v>descriptionlevel supporting collection 0</v>
       </c>
       <c r="L52" t="s">
@@ -2308,7 +2307,7 @@
         <v>72</v>
       </c>
       <c r="C53" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E53,L53)</f>
+        <f t="shared" si="2"/>
         <v>inventorystatus in storage</v>
       </c>
       <c r="D53" t="s">
@@ -2321,7 +2320,7 @@
         <v>14</v>
       </c>
       <c r="K53" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C53,A53)</f>
+        <f t="shared" si="3"/>
         <v>inventorystatus in storage 0</v>
       </c>
       <c r="L53" t="s">
@@ -2336,7 +2335,7 @@
         <v>72</v>
       </c>
       <c r="C54" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E54,L54)</f>
+        <f t="shared" si="2"/>
         <v>inventorystatus missing</v>
       </c>
       <c r="D54" t="s">
@@ -2349,7 +2348,7 @@
         <v>15</v>
       </c>
       <c r="K54" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C54,A54)</f>
+        <f t="shared" si="3"/>
         <v>inventorystatus missing 0</v>
       </c>
       <c r="L54" t="s">
@@ -2364,7 +2363,7 @@
         <v>72</v>
       </c>
       <c r="C55" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E55,L55)</f>
+        <f t="shared" si="2"/>
         <v>inventorystatus off site</v>
       </c>
       <c r="D55" t="s">
@@ -2377,7 +2376,7 @@
         <v>16</v>
       </c>
       <c r="K55" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C55,A55)</f>
+        <f t="shared" si="3"/>
         <v>inventorystatus off site 0</v>
       </c>
       <c r="L55" t="s">
@@ -2392,7 +2391,7 @@
         <v>72</v>
       </c>
       <c r="C56" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E56,L56)</f>
+        <f t="shared" si="2"/>
         <v>inventorystatus removed from collection</v>
       </c>
       <c r="D56" t="s">
@@ -2405,7 +2404,7 @@
         <v>17</v>
       </c>
       <c r="K56" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C56,A56)</f>
+        <f t="shared" si="3"/>
         <v>inventorystatus removed from collection 0</v>
       </c>
       <c r="L56" t="s">
@@ -2420,7 +2419,7 @@
         <v>72</v>
       </c>
       <c r="C57" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E57,L57)</f>
+        <f t="shared" si="2"/>
         <v>nagpracategory undetermined/requires additional consultation</v>
       </c>
       <c r="D57" t="s">
@@ -2433,7 +2432,7 @@
         <v>26</v>
       </c>
       <c r="K57" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C57,A57)</f>
+        <f t="shared" si="3"/>
         <v>nagpracategory undetermined/requires additional consultation 0</v>
       </c>
       <c r="L57" t="s">
@@ -2448,7 +2447,7 @@
         <v>72</v>
       </c>
       <c r="C58" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E58,L58)</f>
+        <f t="shared" si="2"/>
         <v>objectcategory commingled human remains</v>
       </c>
       <c r="D58" t="s">
@@ -2461,7 +2460,7 @@
         <v>40</v>
       </c>
       <c r="K58" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C58,A58)</f>
+        <f t="shared" si="3"/>
         <v>objectcategory commingled human remains 0</v>
       </c>
       <c r="L58" t="s">
@@ -2556,7 +2555,7 @@
         <v>72</v>
       </c>
       <c r="C62" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E62,L62)</f>
+        <f t="shared" ref="C62:C76" si="4">_xlfn.TEXTJOIN(" ",TRUE,E62,L62)</f>
         <v>objectcategory unidentified object</v>
       </c>
       <c r="D62" t="s">
@@ -2569,7 +2568,7 @@
         <v>51</v>
       </c>
       <c r="K62" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C62,A62)</f>
+        <f t="shared" ref="K62:K76" si="5">_xlfn.TEXTJOIN(" ",TRUE,C62,A62)</f>
         <v>objectcategory unidentified object 0</v>
       </c>
       <c r="L62" t="s">
@@ -2584,7 +2583,7 @@
         <v>72</v>
       </c>
       <c r="C63" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E63,L63)</f>
+        <f t="shared" si="4"/>
         <v>organizationtype crm firm</v>
       </c>
       <c r="D63" t="s">
@@ -2597,7 +2596,7 @@
         <v>59</v>
       </c>
       <c r="K63" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C63,A63)</f>
+        <f t="shared" si="5"/>
         <v>organizationtype crm firm 0</v>
       </c>
       <c r="L63" t="s">
@@ -2612,7 +2611,7 @@
         <v>72</v>
       </c>
       <c r="C64" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E64,L64)</f>
+        <f t="shared" si="4"/>
         <v>organizationtype family</v>
       </c>
       <c r="D64" t="s">
@@ -2625,7 +2624,7 @@
         <v>60</v>
       </c>
       <c r="K64" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C64,A64)</f>
+        <f t="shared" si="5"/>
         <v>organizationtype family 0</v>
       </c>
       <c r="L64" t="s">
@@ -2640,7 +2639,7 @@
         <v>72</v>
       </c>
       <c r="C65" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E65,L65)</f>
+        <f t="shared" si="4"/>
         <v>organizationtype federal agency</v>
       </c>
       <c r="D65" t="s">
@@ -2653,7 +2652,7 @@
         <v>61</v>
       </c>
       <c r="K65" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C65,A65)</f>
+        <f t="shared" si="5"/>
         <v>organizationtype federal agency 0</v>
       </c>
       <c r="L65" t="s">
@@ -2668,7 +2667,7 @@
         <v>72</v>
       </c>
       <c r="C66" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E66,L66)</f>
+        <f t="shared" si="4"/>
         <v>organizationtype federally-recognized tribe</v>
       </c>
       <c r="D66" t="s">
@@ -2681,7 +2680,7 @@
         <v>62</v>
       </c>
       <c r="K66" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C66,A66)</f>
+        <f t="shared" si="5"/>
         <v>organizationtype federally-recognized tribe 0</v>
       </c>
       <c r="L66" t="s">
@@ -2696,7 +2695,7 @@
         <v>72</v>
       </c>
       <c r="C67" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E67,L67)</f>
+        <f t="shared" si="4"/>
         <v>organizationtype museum</v>
       </c>
       <c r="D67" t="s">
@@ -2709,7 +2708,7 @@
         <v>63</v>
       </c>
       <c r="K67" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C67,A67)</f>
+        <f t="shared" si="5"/>
         <v>organizationtype museum 0</v>
       </c>
       <c r="L67" t="s">
@@ -2724,7 +2723,7 @@
         <v>72</v>
       </c>
       <c r="C68" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E68,L68)</f>
+        <f t="shared" si="4"/>
         <v>organizationtype non-federally-recognized tribe</v>
       </c>
       <c r="D68" t="s">
@@ -2737,7 +2736,7 @@
         <v>64</v>
       </c>
       <c r="K68" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C68,A68)</f>
+        <f t="shared" si="5"/>
         <v>organizationtype non-federally-recognized tribe 0</v>
       </c>
       <c r="L68" t="s">
@@ -2752,7 +2751,7 @@
         <v>72</v>
       </c>
       <c r="C69" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E69,L69)</f>
+        <f t="shared" si="4"/>
         <v>publishto CollectionSpace Public Browser</v>
       </c>
       <c r="D69" t="s">
@@ -2765,7 +2764,7 @@
         <v>67</v>
       </c>
       <c r="K69" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C69,A69)</f>
+        <f t="shared" si="5"/>
         <v>publishto CollectionSpace Public Browser 0</v>
       </c>
       <c r="L69" t="s">
@@ -2780,7 +2779,7 @@
         <v>72</v>
       </c>
       <c r="C70" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E70,L70)</f>
+        <f t="shared" si="4"/>
         <v>publishto None</v>
       </c>
       <c r="D70" t="s">
@@ -2793,7 +2792,7 @@
         <v>68</v>
       </c>
       <c r="K70" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C70,A70)</f>
+        <f t="shared" si="5"/>
         <v>publishto None 0</v>
       </c>
       <c r="L70" t="s">
@@ -2808,7 +2807,7 @@
         <v>74</v>
       </c>
       <c r="C71" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E71,L71)</f>
+        <f t="shared" si="4"/>
         <v>publishto None</v>
       </c>
       <c r="D71" t="s">
@@ -2821,7 +2820,7 @@
         <v>79</v>
       </c>
       <c r="K71" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C71,A71)</f>
+        <f t="shared" si="5"/>
         <v>publishto None 1</v>
       </c>
       <c r="L71" t="s">
@@ -2836,7 +2835,7 @@
         <v>72</v>
       </c>
       <c r="C72" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E72,L72)</f>
+        <f t="shared" si="4"/>
         <v>publishto Omeka</v>
       </c>
       <c r="D72" t="s">
@@ -2849,7 +2848,7 @@
         <v>77</v>
       </c>
       <c r="K72" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C72,A72)</f>
+        <f t="shared" si="5"/>
         <v>publishto Omeka 0</v>
       </c>
       <c r="L72" t="s">
@@ -2864,7 +2863,7 @@
         <v>78</v>
       </c>
       <c r="C73" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E73,L73)</f>
+        <f t="shared" si="4"/>
         <v>publishto Omeka</v>
       </c>
       <c r="D73" t="s">
@@ -2877,7 +2876,7 @@
         <v>77</v>
       </c>
       <c r="K73" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C73,A73)</f>
+        <f t="shared" si="5"/>
         <v>publishto Omeka 2</v>
       </c>
       <c r="L73" t="s">
@@ -2892,24 +2891,24 @@
         <v>72</v>
       </c>
       <c r="C74" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E74,L74)</f>
+        <f t="shared" si="4"/>
         <v>newvocab Term 1</v>
       </c>
       <c r="D74" t="s">
+        <v>123</v>
+      </c>
+      <c r="E74" t="s">
         <v>124</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>125</v>
       </c>
-      <c r="F74" t="s">
-        <v>126</v>
-      </c>
-      <c r="K74" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C74,A74)</f>
+      <c r="K74" t="str">
+        <f t="shared" si="5"/>
         <v>newvocab Term 1 4</v>
       </c>
       <c r="L74" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
@@ -2920,24 +2919,24 @@
         <v>72</v>
       </c>
       <c r="C75" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E75,L75)</f>
+        <f t="shared" si="4"/>
         <v>newvocab Term 2</v>
       </c>
       <c r="D75" t="s">
+        <v>123</v>
+      </c>
+      <c r="E75" t="s">
         <v>124</v>
       </c>
-      <c r="E75" t="s">
-        <v>125</v>
-      </c>
       <c r="F75" t="s">
-        <v>127</v>
-      </c>
-      <c r="K75" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C75,A75)</f>
+        <v>126</v>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="5"/>
         <v>newvocab Term 2 4</v>
       </c>
       <c r="L75" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
@@ -2948,24 +2947,24 @@
         <v>72</v>
       </c>
       <c r="C76" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,E76,L76)</f>
+        <f t="shared" si="4"/>
         <v>newvocab Term 3</v>
       </c>
       <c r="D76" t="s">
+        <v>123</v>
+      </c>
+      <c r="E76" t="s">
         <v>124</v>
       </c>
-      <c r="E76" t="s">
-        <v>125</v>
-      </c>
       <c r="F76" t="s">
-        <v>128</v>
-      </c>
-      <c r="K76" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,C76,A76)</f>
+        <v>127</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="5"/>
         <v>newvocab Term 3 4</v>
       </c>
       <c r="L76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2987,6 +2986,25 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9ecaf8b9-395e-4614-9554-a754ef4fa6ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3e0fc0fe-d5d6-438e-8bc4-7eae18f70edf" xsi:nil="true"/>
+    <LocalDescription xmlns="9ecaf8b9-395e-4614-9554-a754ef4fa6ce" xsi:nil="true"/>
+    <SharedWithUsers xmlns="3e0fc0fe-d5d6-438e-8bc4-7eae18f70edf">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A00C4DE627EB54449BA92EDD4203D684" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4c66ae8ad5e806d130737f1340b5989e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ecaf8b9-395e-4614-9554-a754ef4fa6ce" xmlns:ns3="3e0fc0fe-d5d6-438e-8bc4-7eae18f70edf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37a5a0aced1fd5955e1b293c1cac970c" ns2:_="" ns3:_="">
     <xsd:import namespace="9ecaf8b9-395e-4614-9554-a754ef4fa6ce"/>
@@ -3231,25 +3249,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9ecaf8b9-395e-4614-9554-a754ef4fa6ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3e0fc0fe-d5d6-438e-8bc4-7eae18f70edf" xsi:nil="true"/>
-    <LocalDescription xmlns="9ecaf8b9-395e-4614-9554-a754ef4fa6ce" xsi:nil="true"/>
-    <SharedWithUsers xmlns="3e0fc0fe-d5d6-438e-8bc4-7eae18f70edf">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{745D81CB-460C-442A-83F1-2C1DC7BE8992}">
   <ds:schemaRefs>
@@ -3259,6 +3258,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EDFA113-67C1-4162-9EA5-E3D1ED29EBCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="9ecaf8b9-395e-4614-9554-a754ef4fa6ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e0fc0fe-d5d6-438e-8bc4-7eae18f70edf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{181D3AEF-658E-48AA-B8AE-644B198301DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3275,21 +3291,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EDFA113-67C1-4162-9EA5-E3D1ED29EBCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="9ecaf8b9-395e-4614-9554-a754ef4fa6ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e0fc0fe-d5d6-438e-8bc4-7eae18f70edf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>